<commit_message>
complete smoke & sanity on Login page- hms dated on 23/10/2018 by sanket
</commit_message>
<xml_diff>
--- a/hms/resources/utils/User.xlsx
+++ b/hms/resources/utils/User.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13785" windowHeight="10620" tabRatio="296" firstSheet="2"/>
+    <workbookView windowWidth="13785" windowHeight="4905" tabRatio="296" firstSheet="2" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="validusers" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
   <si>
     <t>UserName</t>
   </si>
@@ -36,16 +36,19 @@
     <t>Invalid Passwords</t>
   </si>
   <si>
+    <t>Admin$123456789</t>
+  </si>
+  <si>
     <t>tsethms2@@mailinator.com</t>
   </si>
   <si>
     <t>Admin$123</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
+    <t xml:space="preserve">                                                          </t>
   </si>
   <si>
-    <t xml:space="preserve">     </t>
+    <t xml:space="preserve">                       </t>
   </si>
 </sst>
 </file>
@@ -53,10 +56,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -76,15 +79,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -92,6 +87,28 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -105,6 +122,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -113,101 +199,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -220,43 +223,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,49 +367,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,85 +391,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,6 +414,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -438,6 +456,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -453,17 +486,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -485,38 +514,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -534,130 +537,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -995,8 +998,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1035,8 +1038,8 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="$A7:$XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1057,24 +1060,24 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>12345678</v>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1082,14 +1085,14 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="testhms1@mailinator.com"/>
+    <hyperlink ref="A5" r:id="rId1" display="testhms1@mailinator.com"/>
     <hyperlink ref="A3" r:id="rId2" display="tsethms2@@mailinator.com" tooltip="mailto:tsethms2@@mailinator.com"/>
-    <hyperlink ref="A5" r:id="rId1" display="testhms1@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
database connection using static blocks by sanket @29/10/2018
</commit_message>
<xml_diff>
--- a/hms/resources/utils/User.xlsx
+++ b/hms/resources/utils/User.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13785" windowHeight="4905" tabRatio="296" firstSheet="2" activeTab="1"/>
+    <workbookView windowWidth="14700" windowHeight="8070" tabRatio="296" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="validusers" sheetId="1" r:id="rId1"/>
     <sheet name="invalidusers" sheetId="2" r:id="rId2"/>
+    <sheet name="database" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:B5"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>UserName</t>
   </si>
@@ -49,6 +50,42 @@
   </si>
   <si>
     <t xml:space="preserve">                       </t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>databasename</t>
+  </si>
+  <si>
+    <t>database_url</t>
+  </si>
+  <si>
+    <t>driver type</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>3306</t>
+  </si>
+  <si>
+    <t>hms_db</t>
+  </si>
+  <si>
+    <t>jdbc:mysql://192.168.1.120</t>
+  </si>
+  <si>
+    <t>com.mysql.cj.jdbc.Driver</t>
   </si>
 </sst>
 </file>
@@ -56,10 +93,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -78,6 +115,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,32 +145,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -123,7 +162,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,6 +170,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -139,53 +208,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,17 +223,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -223,25 +260,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,157 +434,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,17 +469,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -452,21 +483,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,6 +504,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -497,20 +537,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -519,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -537,130 +574,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1038,8 +1075,8 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="$A7:$XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1097,4 +1134,68 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="15.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="18.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="11.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="39.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new changes in forgot password pom @16/11/2018
</commit_message>
<xml_diff>
--- a/hms/resources/utils/User.xlsx
+++ b/hms/resources/utils/User.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14700" windowHeight="8070" tabRatio="296" firstSheet="2" activeTab="2"/>
+    <workbookView windowWidth="14445" windowHeight="6945" tabRatio="296" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="validusers" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
   <si>
     <t>UserName</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">                       </t>
+  </si>
+  <si>
+    <t>testhms2@mailinator.comom</t>
   </si>
   <si>
     <t>username</t>
@@ -93,10 +96,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -110,6 +113,118 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,21 +238,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -145,107 +246,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,187 +263,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,6 +454,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -474,30 +516,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,27 +554,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -574,130 +577,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1073,13 +1076,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="$A9:$XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="33.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="32.4285714285714" customWidth="1"/>
@@ -1125,11 +1128,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="testhms1@mailinator.com"/>
     <hyperlink ref="A5" r:id="rId1" display="testhms1@mailinator.com"/>
     <hyperlink ref="A3" r:id="rId2" display="tsethms2@@mailinator.com" tooltip="mailto:tsethms2@@mailinator.com"/>
+    <hyperlink ref="A6" r:id="rId3" display="testhms2@mailinator.comom" tooltip="mailto:testhms2@mailinator.comom"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1141,7 +1153,7 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1156,42 +1168,42 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test data created for private practitioner @05122018 EOD
</commit_message>
<xml_diff>
--- a/hms/resources/utils/User.xlsx
+++ b/hms/resources/utils/User.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18000" windowHeight="10620" tabRatio="296" firstSheet="3" activeTab="4"/>
+    <workbookView windowWidth="13785" windowHeight="5520" tabRatio="296" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="validusers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171">
   <si>
     <t>UserName</t>
   </si>
@@ -169,6 +169,9 @@
     <t>02046525</t>
   </si>
   <si>
+    <t>99758445685</t>
+  </si>
+  <si>
     <t>rama pride</t>
   </si>
   <si>
@@ -181,9 +184,15 @@
     <t>pune</t>
   </si>
   <si>
+    <t>411033</t>
+  </si>
+  <si>
     <t>01121990</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>testhms5@mailinator.com</t>
   </si>
   <si>
@@ -196,42 +205,90 @@
     <t>BAMS</t>
   </si>
   <si>
+    <t>2006</t>
+  </si>
+  <si>
     <t>Current</t>
   </si>
   <si>
+    <t>1024568254</t>
+  </si>
+  <si>
     <t>Maharashtra council</t>
   </si>
   <si>
+    <t>2007</t>
+  </si>
+  <si>
     <t>02046526</t>
   </si>
   <si>
+    <t>411034</t>
+  </si>
+  <si>
     <t>01121991</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>testhms6@mailinator.com</t>
   </si>
   <si>
+    <t>1024568255</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
     <t>02046527</t>
   </si>
   <si>
+    <t>411035</t>
+  </si>
+  <si>
     <t>01121992</t>
   </si>
   <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>testhms7@mailinator.com</t>
   </si>
   <si>
+    <t>1024568256</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
     <t>02046528</t>
   </si>
   <si>
+    <t>411036</t>
+  </si>
+  <si>
     <t>01121993</t>
   </si>
   <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>testhms8@mailinator.com</t>
   </si>
   <si>
+    <t>1024568257</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
     <t xml:space="preserve">caption character limit is  caption character limit is  caption character limit is </t>
   </si>
   <si>
+    <t>123456789</t>
+  </si>
+  <si>
     <t>99758445685020</t>
   </si>
   <si>
@@ -241,6 +298,12 @@
     <t>dattcaption character limit is 255 caption character limit is  caption character limit is caption character limit is 255 caption character limit is  caption character limit is caption character limit is 255 caption character limit is  caption character limit is awadi road</t>
   </si>
   <si>
+    <t>411033000</t>
+  </si>
+  <si>
+    <t>2223</t>
+  </si>
+  <si>
     <t>1111111111111111111111111111111111111222222222222222222222222222222222</t>
   </si>
   <si>
@@ -289,12 +352,30 @@
     <t>caption character limit is two hundredscaption character limit is two hundredscaption character limit is two hundredscaption character limit is two hundredscaption character limit is two hundredscaption character limit is two hundreds</t>
   </si>
   <si>
+    <t>20198</t>
+  </si>
+  <si>
     <t>@134$123</t>
   </si>
   <si>
     <t>@134$124</t>
   </si>
   <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>123457</t>
+  </si>
+  <si>
+    <t>123458</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
     <t>Telangana</t>
   </si>
   <si>
@@ -304,7 +385,7 @@
     <t>#po123</t>
   </si>
   <si>
-    <t xml:space="preserve">     </t>
+    <t>01121994</t>
   </si>
   <si>
     <t>#123</t>
@@ -316,9 +397,15 @@
     <t>Gynaecologist</t>
   </si>
   <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
     <t>0000</t>
   </si>
   <si>
+    <t>Expired</t>
+  </si>
+  <si>
     <t>BU-302</t>
   </si>
   <si>
@@ -337,40 +424,28 @@
     <t>Ahmedabad</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">       </t>
+    <t>123</t>
+  </si>
+  <si>
+    <t>23yr</t>
+  </si>
+  <si>
+    <t>#198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t>state_name</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
   </si>
   <si>
     <t>West Bengal</t>
-  </si>
-  <si>
-    <t>Darjiling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         </t>
-  </si>
-  <si>
-    <t>01121994</t>
-  </si>
-  <si>
-    <t>Ophthalmologist</t>
-  </si>
-  <si>
-    <t>#198</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          </t>
-  </si>
-  <si>
-    <t>state_name</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
   </si>
   <si>
     <t>Rajasthan</t>
@@ -466,9 +541,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -516,15 +591,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -561,23 +628,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,10 +667,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -607,8 +682,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,9 +697,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -635,13 +717,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -652,12 +727,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -670,13 +781,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,151 +901,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -897,6 +972,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -914,30 +1013,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -948,7 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -966,37 +1041,37 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1008,88 +1083,88 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1105,19 +1180,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="10" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="10" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
@@ -1463,7 +1535,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1503,7 +1575,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1511,7 +1583,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -1527,7 +1599,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -1535,7 +1607,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
@@ -1624,356 +1696,358 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="15.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="15.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="15.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="18.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="20.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="18.4285714285714" customWidth="1"/>
-    <col min="7" max="7" width="19.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="16.4285714285714" customWidth="1"/>
-    <col min="9" max="9" width="12.4285714285714" customWidth="1"/>
-    <col min="10" max="10" width="11.4285714285714" customWidth="1"/>
-    <col min="11" max="11" width="10.1428571428571" customWidth="1"/>
-    <col min="12" max="12" width="23.2857142857143" customWidth="1"/>
-    <col min="13" max="13" width="23.1428571428571" customWidth="1"/>
-    <col min="14" max="14" width="21.2857142857143" customWidth="1"/>
-    <col min="15" max="15" width="20.7142857142857" customWidth="1"/>
-    <col min="17" max="17" width="11.4285714285714" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="16.7142857142857" customWidth="1"/>
-    <col min="20" max="20" width="14.1428571428571" customWidth="1"/>
-    <col min="21" max="21" width="16.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="15.7142857142857" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.1428571428571" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.8571428571429" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.5714285714286" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.4285714285714" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.4285714285714" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.8571428571429" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.4285714285714" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.4285714285714" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.4285714285714" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.1428571428571" style="4" customWidth="1"/>
+    <col min="12" max="12" width="23.2857142857143" style="4" customWidth="1"/>
+    <col min="13" max="13" width="23.1428571428571" style="4" customWidth="1"/>
+    <col min="14" max="14" width="21.2857142857143" style="4" customWidth="1"/>
+    <col min="15" max="15" width="20.7142857142857" style="4" customWidth="1"/>
+    <col min="16" max="16" width="9.14285714285714" style="4"/>
+    <col min="17" max="17" width="11.4285714285714" style="4" customWidth="1"/>
+    <col min="18" max="18" width="15" style="4" customWidth="1"/>
+    <col min="19" max="19" width="16.7142857142857" style="4" customWidth="1"/>
+    <col min="20" max="20" width="14.1428571428571" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.2857142857143" style="4" customWidth="1"/>
+    <col min="22" max="16384" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" ht="30" spans="1:21">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="3" customFormat="1" ht="30" spans="1:21">
+      <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E2">
-        <v>99758445685</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J2">
-        <v>411033</v>
+      <c r="I2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L2">
-        <v>20</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2">
-        <v>2006</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="J3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="S2">
-        <v>1024568254</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="O3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="U2">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" t="s">
+      <c r="P3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E3">
-        <v>99758445686</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="Q4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J3">
-        <v>411034</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3">
-        <v>21</v>
-      </c>
-      <c r="M3" s="7" t="s">
+      <c r="I5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="N3" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q3">
-        <v>2007</v>
-      </c>
-      <c r="R3" t="s">
-        <v>58</v>
-      </c>
-      <c r="S3">
-        <v>1024568255</v>
-      </c>
-      <c r="T3" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4">
-        <v>99758445687</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4">
-        <v>411035</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="S5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="T5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L4">
-        <v>22</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="N4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4">
-        <v>2008</v>
-      </c>
-      <c r="R4" t="s">
-        <v>58</v>
-      </c>
-      <c r="S4">
-        <v>1024568256</v>
-      </c>
-      <c r="T4" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5">
-        <v>99758445688</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5">
-        <v>411036</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5">
-        <v>23</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="N5" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q5">
-        <v>2009</v>
-      </c>
-      <c r="R5" t="s">
-        <v>58</v>
-      </c>
-      <c r="S5">
-        <v>1024568257</v>
-      </c>
-      <c r="T5" t="s">
-        <v>59</v>
-      </c>
-      <c r="U5">
-        <v>2010</v>
+      <c r="U5" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2002,13 +2076,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="$A16:$XFD16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="15.1428571428571" style="4" customWidth="1"/>
     <col min="2" max="2" width="15.8571428571429" style="4" customWidth="1"/>
@@ -2093,259 +2167,259 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="4" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="4">
-        <v>123456789</v>
+        <v>87</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="4">
-        <v>411033000</v>
+        <v>53</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="4">
-        <v>2223</v>
-      </c>
-      <c r="M2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>20</v>
-      </c>
       <c r="R2" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="U2" s="4">
-        <v>20</v>
+        <v>95</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>78</v>
+        <v>98</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>86</v>
+        <v>106</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>20198</v>
+        <v>109</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" s="4">
-        <v>20198</v>
+        <v>112</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="4">
-        <v>123456</v>
-      </c>
-      <c r="B4" s="4">
-        <v>123457</v>
-      </c>
-      <c r="C4" s="4">
-        <v>123458</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1234567</v>
-      </c>
-      <c r="E4" s="4">
-        <v>12345</v>
+      <c r="A4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>93</v>
+        <v>119</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>94</v>
+        <v>124</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="4">
+        <v>133</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="N5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>94</v>
+        <v>58</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="U5" s="4" t="s">
         <v>40</v>
@@ -2353,137 +2427,75 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>110</v>
+        <v>125</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>94</v>
+        <v>123</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5">
       <formula1>states!$A$2:$A$37</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5">
       <formula1>"Cardiologist,Dermatologist,Gynaecologist,Ophthalmologist"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R6">
@@ -2512,187 +2524,187 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="2" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="2" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="2" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="2" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="2" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
capture screenshot implemented @18012019
</commit_message>
<xml_diff>
--- a/hms/resources/utils/User.xlsx
+++ b/hms/resources/utils/User.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15015" windowHeight="9060" tabRatio="296" firstSheet="1" activeTab="3"/>
+    <workbookView windowWidth="9810" windowHeight="6285" tabRatio="296"/>
   </bookViews>
   <sheets>
     <sheet name="validusers" sheetId="1" r:id="rId1"/>
@@ -28,27 +28,27 @@
     <t>Passwords</t>
   </si>
   <si>
+    <t>hms_admin1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Admin$123</t>
+  </si>
+  <si>
+    <t>Invalid UserName</t>
+  </si>
+  <si>
+    <t>Invalid Passwords</t>
+  </si>
+  <si>
     <t>testhms1@mailinator.com</t>
   </si>
   <si>
-    <t>Password$123</t>
-  </si>
-  <si>
-    <t>Invalid UserName</t>
-  </si>
-  <si>
-    <t>Invalid Passwords</t>
-  </si>
-  <si>
     <t>Admin$123456789</t>
   </si>
   <si>
     <t>tsethms2@@mailinator.com</t>
   </si>
   <si>
-    <t>Admin$123</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                          </t>
   </si>
   <si>
@@ -193,7 +193,7 @@
     <t>20</t>
   </si>
   <si>
-    <t>testhms5@mailinator.com</t>
+    <t>testhmsPP5@mailinator.com</t>
   </si>
   <si>
     <t>Cardiologist</t>
@@ -232,7 +232,7 @@
     <t>21</t>
   </si>
   <si>
-    <t>testhms6@mailinator.com</t>
+    <t>testhmsPP6@mailinator.com</t>
   </si>
   <si>
     <t>1024568255</t>
@@ -253,7 +253,7 @@
     <t>22</t>
   </si>
   <si>
-    <t>testhms7@mailinator.com</t>
+    <t>testhmsPP7@mailinator.com</t>
   </si>
   <si>
     <t>1024568256</t>
@@ -274,7 +274,7 @@
     <t>23</t>
   </si>
   <si>
-    <t>testhms8@mailinator.com</t>
+    <t>testhmsPP8@mailinator.com</t>
   </si>
   <si>
     <t>1024568257</t>
@@ -541,9 +541,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -591,7 +591,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -604,8 +634,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -619,32 +673,22 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -659,33 +703,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -696,27 +717,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -727,19 +727,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,19 +823,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,139 +901,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,21 +936,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -962,11 +947,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,9 +986,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1013,8 +1013,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1023,7 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1041,130 +1041,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1516,8 +1516,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="$A5:$XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1544,7 +1544,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="testhms1@mailinator.com" tooltip="mailto:testhms1@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="hms_admin1@mailinator.com" tooltip="mailto:hms_admin1@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1576,18 +1576,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1595,12 +1595,12 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1631,8 +1631,8 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1695,7 +1695,7 @@
   <sheetPr/>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2063,10 +2063,10 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="testhms5@mailinator.com"/>
-    <hyperlink ref="M3" r:id="rId1" display="testhms6@mailinator.com"/>
-    <hyperlink ref="M4" r:id="rId1" display="testhms7@mailinator.com"/>
-    <hyperlink ref="M5" r:id="rId1" display="testhms8@mailinator.com"/>
+    <hyperlink ref="M2" r:id="rId1" display="testhmsPP5@mailinator.com" tooltip="mailto:testhmsPP5@mailinator.com"/>
+    <hyperlink ref="M3" r:id="rId1" display="testhmsPP6@mailinator.com" tooltip="mailto:testhmsPP5@mailinator.com"/>
+    <hyperlink ref="M4" r:id="rId1" display="testhmsPP7@mailinator.com" tooltip="mailto:testhmsPP5@mailinator.com"/>
+    <hyperlink ref="M5" r:id="rId1" display="testhmsPP8@mailinator.com" tooltip="mailto:testhmsPP5@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -2078,8 +2078,8 @@
   <sheetPr/>
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -2203,7 +2203,7 @@
         <v>93</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>58</v>
@@ -2516,7 +2516,7 @@
   <sheetPr/>
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:A37"/>
     </sheetView>
   </sheetViews>

</xml_diff>